<commit_message>
Add Risks packages and update AI_Risk_Assessment_Guide.xlsx
</commit_message>
<xml_diff>
--- a/AI_Risk_Assessment_Guide.xlsx
+++ b/AI_Risk_Assessment_Guide.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtmastercarbonfr-my.sharepoint.com/personal/mia_dtmastercarbon_fr/Documents/DT Master Mia Personal/5 Tech/AI act/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miachen/Desktop/Mia/DT Master/Tech/Hackthon/geminihackathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="11_4574718D76E88B084351573C1EA557AA9DB44E10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E640AA22-A95C-AF40-9C19-F3A470F8A7EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF73E99-26B6-164C-85E3-4E1E77D5E04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="500" windowWidth="33600" windowHeight="19580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34180" yWindow="500" windowWidth="33600" windowHeight="19580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
-    <sheet name="High-Risk Gap Analysis" sheetId="1" r:id="rId2"/>
+    <sheet name="New functionnality" sheetId="11" r:id="rId2"/>
     <sheet name="Risk Tools" sheetId="4" r:id="rId3"/>
     <sheet name="No compulsory" sheetId="5" r:id="rId4"/>
     <sheet name="Risk-Tool Mapping" sheetId="6" r:id="rId5"/>
@@ -24,7 +24,7 @@
     <sheet name="Risk Taxonomy" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'High-Risk Gap Analysis'!$A$1:$K$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'New functionnality'!$A$1:$K$44</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Risk Tools'!$A$1:$R$132</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3937" uniqueCount="1872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3939" uniqueCount="1872">
   <si>
     <t>Category</t>
   </si>
@@ -5660,14 +5660,14 @@
     <t>UI UX Front</t>
   </si>
   <si>
-    <t>Johnny or Christophe</t>
+    <t>Yuan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5751,13 +5751,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5962,19 +5955,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5991,22 +5974,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -6021,8 +5995,27 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6340,12 +6333,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6467,1566 +6460,1575 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3987F22-779D-9647-9276-649C25B39FCD}">
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="39" customWidth="1"/>
-    <col min="5" max="5" width="30" style="39" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="33" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="50" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="50" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
     <col min="10" max="10" width="40" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="34" t="s">
         <v>1262</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="34" t="s">
         <v>1867</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="34" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="34"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="32" t="s">
         <v>900</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="28"/>
+      <c r="B3" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D3" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="28"/>
+      <c r="B4" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="28"/>
+      <c r="B5" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="28"/>
+      <c r="B6" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="32" t="s">
+        <v>900</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="35" t="s">
+        <v>729</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>566</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="28"/>
+      <c r="B13" s="35" t="s">
+        <v>729</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" s="35" t="s">
+        <v>729</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="D16" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E16" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="28" t="s">
+      <c r="G16" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J16" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K16" s="27" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="38" t="s">
+    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>381</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="28"/>
+      <c r="B24" s="49" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="28"/>
+      <c r="B25" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A26" s="28"/>
+      <c r="B26" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>566</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="28"/>
+      <c r="B27" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>566</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="G27" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A28" s="28"/>
+      <c r="B28" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="G28" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="28"/>
+      <c r="B30" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A31" s="28"/>
+      <c r="B31" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>1868</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="K31" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="28"/>
+      <c r="B33" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="28"/>
+      <c r="B34" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="28"/>
+      <c r="B35" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A36" s="28"/>
+      <c r="B36" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A37" s="28"/>
+      <c r="B37" s="30" t="s">
+        <v>715</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="28"/>
+      <c r="B38" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="28"/>
+      <c r="B39" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="28"/>
+      <c r="B40" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="J40" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K40" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="28"/>
+      <c r="B41" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="28"/>
+      <c r="B42" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="G42" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="J42" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="K42" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A43" s="28"/>
+      <c r="B43" s="40" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D43" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E43" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="G43" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" s="27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="28"/>
+      <c r="B44" s="40" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>804</v>
+      </c>
+      <c r="D44" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="31"/>
+      <c r="C50" s="31" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="31" t="s">
+        <v>898</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="32" t="s">
         <v>900</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>192</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="34"/>
-      <c r="B4" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="34"/>
-      <c r="B5" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="34"/>
-      <c r="B6" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>415</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="J6" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>415</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="34"/>
-      <c r="B8" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>415</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="K8" s="28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" s="34"/>
-      <c r="B9" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>415</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="37" t="s">
+      <c r="C52" s="31">
+        <f t="shared" ref="C52:C60" si="0">COUNTIF($B$4:$B$44,B52)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53" s="29" t="s">
+        <v>896</v>
+      </c>
+      <c r="C53" s="31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54" s="31" t="s">
+        <v>715</v>
+      </c>
+      <c r="C54" s="31">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55" s="38" t="s">
+        <v>882</v>
+      </c>
+      <c r="C55" s="31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56" s="31" t="s">
         <v>603</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D10" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="37" t="s">
-        <v>603</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D11" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="34"/>
-      <c r="B12" s="37" t="s">
-        <v>603</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D12" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="J12" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="K12" s="28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="37" t="s">
-        <v>603</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="K13" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="34"/>
-      <c r="B14" s="43" t="s">
+      <c r="C56" s="31">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57" s="39" t="s">
+        <v>594</v>
+      </c>
+      <c r="C57" s="31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58" s="35" t="s">
         <v>729</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>566</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="E14" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="J14" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="K14" s="28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="43" t="s">
-        <v>729</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E15" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="K15" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="34"/>
-      <c r="B16" s="43" t="s">
-        <v>729</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>415</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>242</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>243</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="J16" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="K16" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C17" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="K17" s="28" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E18" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I18" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="K18" s="28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
-      <c r="B20" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="K20" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35" t="s">
+      <c r="C58" s="31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="40" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C59" s="31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="49" t="s">
         <v>1871</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D21" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" s="46" t="s">
-        <v>155</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="G21" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="K21" s="28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35" t="s">
-        <v>1871</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="28" t="s">
-        <v>162</v>
-      </c>
-      <c r="J22" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="K22" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>381</v>
-      </c>
-      <c r="D23" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="E23" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="K23" s="28" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="34"/>
-      <c r="B24" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>1869</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>231</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I24" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="K24" s="28" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="34"/>
-      <c r="B25" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>1869</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="E25" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I25" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="J25" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="K25" s="28" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="34"/>
-      <c r="B26" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>566</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="F26" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I26" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="J26" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="K26" s="28" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="34"/>
-      <c r="B27" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>566</v>
-      </c>
-      <c r="D27" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E27" s="46" t="s">
-        <v>177</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="G27" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="K27" s="28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D28" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>213</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="48" t="s">
-        <v>594</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>1868</v>
-      </c>
-      <c r="D29" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="K29" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
-      <c r="B30" s="48" t="s">
-        <v>594</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>1868</v>
-      </c>
-      <c r="D30" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I30" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="J30" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="K30" s="28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="48" t="s">
-        <v>594</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>1868</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="K31" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="F32" s="28" t="s">
-        <v>166</v>
-      </c>
-      <c r="G32" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="K32" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D33" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="F33" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I33" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="J33" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
-      <c r="B34" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I34" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="J34" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D35" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H35" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I35" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K35" s="28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C36" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D36" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="J36" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="K36" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="36" t="s">
-        <v>715</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D37" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G37" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I37" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="K37" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
-      <c r="B38" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K38" s="28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="34"/>
-      <c r="B39" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I39" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="J39" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39" s="28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
-      <c r="B40" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I40" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="J40" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="K40" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="48" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
-      <c r="B41" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="F41" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="J41" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="K41" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="32" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34"/>
-      <c r="B42" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="E42" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="J42" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="K42" s="28" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A43" s="34"/>
-      <c r="B43" s="49" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>201</v>
-      </c>
-      <c r="F43" s="28" t="s">
-        <v>202</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I43" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="J43" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="K43" s="28" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
-      <c r="B44" s="49" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I44" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="J44" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="K44" s="28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B50" s="37"/>
-      <c r="C50" s="40" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B51" s="37" t="s">
-        <v>898</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>1870</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B52" s="38" t="s">
-        <v>900</v>
-      </c>
-      <c r="C52" s="40">
-        <f>COUNTIF($B$4:$B$44,B52)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B53" s="35" t="s">
-        <v>896</v>
-      </c>
-      <c r="C53" s="40">
-        <f>COUNTIF($B$4:$B$44,B53)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="37" t="s">
-        <v>715</v>
-      </c>
-      <c r="C54" s="40">
-        <f>COUNTIF($B$4:$B$44,B54)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B55" s="47" t="s">
-        <v>882</v>
-      </c>
-      <c r="C55" s="40">
-        <f>COUNTIF($B$4:$B$44,B55)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B56" s="37" t="s">
-        <v>603</v>
-      </c>
-      <c r="C56" s="40">
-        <f>COUNTIF($B$4:$B$44,B56)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="48" t="s">
-        <v>594</v>
-      </c>
-      <c r="C57" s="40">
-        <f>COUNTIF($B$4:$B$44,B57)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B58" s="43" t="s">
-        <v>729</v>
-      </c>
-      <c r="C58" s="40">
-        <f>COUNTIF($B$4:$B$44,B58)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B59" s="49" t="s">
-        <v>1866</v>
-      </c>
-      <c r="C59" s="40">
-        <f>COUNTIF($B$4:$B$44,B59)</f>
-        <v>2</v>
+      <c r="C60" s="31">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -8037,23 +8039,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView topLeftCell="B78" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="35" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="35" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="57.83203125" customWidth="1"/>
     <col min="11" max="11" width="117" customWidth="1"/>
     <col min="12" max="12" width="73.33203125" bestFit="1" customWidth="1"/>
@@ -8196,7 +8199,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -8237,7 +8240,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -8278,7 +8281,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>289</v>
       </c>
@@ -8319,7 +8322,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>289</v>
       </c>
@@ -8360,7 +8363,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -8402,7 +8405,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -8443,7 +8446,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -8484,7 +8487,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>154</v>
       </c>
@@ -8566,7 +8569,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
@@ -8607,7 +8610,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -8648,7 +8651,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -8689,7 +8692,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -8730,7 +8733,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -8777,7 +8780,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>381</v>
       </c>
@@ -8818,7 +8821,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>381</v>
       </c>
@@ -8859,7 +8862,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>381</v>
       </c>
@@ -8900,7 +8903,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>381</v>
       </c>
@@ -8941,7 +8944,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>381</v>
       </c>
@@ -8982,7 +8985,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>381</v>
       </c>
@@ -9023,7 +9026,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>415</v>
       </c>
@@ -9064,7 +9067,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>415</v>
       </c>
@@ -9105,7 +9108,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>415</v>
       </c>
@@ -9146,7 +9149,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>415</v>
       </c>
@@ -9187,7 +9190,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>415</v>
       </c>
@@ -9228,7 +9231,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>415</v>
       </c>
@@ -9269,7 +9272,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>415</v>
       </c>
@@ -9310,7 +9313,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>415</v>
       </c>
@@ -9351,7 +9354,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>459</v>
       </c>
@@ -9392,7 +9395,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>459</v>
       </c>
@@ -9433,7 +9436,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>459</v>
       </c>
@@ -9474,7 +9477,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>459</v>
       </c>
@@ -9515,7 +9518,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>459</v>
       </c>
@@ -9556,7 +9559,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>459</v>
       </c>
@@ -9597,7 +9600,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -9638,7 +9641,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -9679,7 +9682,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -9720,7 +9723,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -9761,7 +9764,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -9802,7 +9805,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -9849,7 +9852,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>528</v>
       </c>
@@ -9890,7 +9893,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>528</v>
       </c>
@@ -9931,7 +9934,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>528</v>
       </c>
@@ -9972,7 +9975,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>528</v>
       </c>
@@ -10013,7 +10016,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>528</v>
       </c>
@@ -10054,7 +10057,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>528</v>
       </c>
@@ -10095,7 +10098,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>528</v>
       </c>
@@ -10137,7 +10140,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>566</v>
       </c>
@@ -10178,7 +10181,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>566</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>566</v>
       </c>
@@ -10260,7 +10263,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>566</v>
       </c>
@@ -10301,7 +10304,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>566</v>
       </c>
@@ -10342,7 +10345,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>566</v>
       </c>
@@ -10442,7 +10445,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>566</v>
       </c>
@@ -10482,7 +10485,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>617</v>
       </c>
@@ -10524,7 +10527,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>617</v>
       </c>
@@ -10566,7 +10569,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>617</v>
       </c>
@@ -10605,7 +10608,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>617</v>
       </c>
@@ -10647,7 +10650,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>617</v>
       </c>
@@ -10689,7 +10692,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>617</v>
       </c>
@@ -10731,7 +10734,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>617</v>
       </c>
@@ -10781,7 +10784,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>661</v>
       </c>
@@ -10824,7 +10827,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>661</v>
       </c>
@@ -10874,8 +10877,11 @@
       <c r="B68" s="21" t="s">
         <v>662</v>
       </c>
+      <c r="C68" s="21" t="s">
+        <v>714</v>
+      </c>
       <c r="D68" s="21" t="s">
-        <v>594</v>
+        <v>715</v>
       </c>
       <c r="F68" s="23" t="s">
         <v>673</v>
@@ -10917,7 +10923,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>661</v>
       </c>
@@ -10960,7 +10966,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>661</v>
       </c>
@@ -10999,7 +11005,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>691</v>
       </c>
@@ -11041,7 +11047,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>691</v>
       </c>
@@ -11083,7 +11089,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>691</v>
       </c>
@@ -11125,7 +11131,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>691</v>
       </c>
@@ -11217,7 +11223,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>691</v>
       </c>
@@ -11314,7 +11320,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="78" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="23" t="s">
         <v>739</v>
       </c>
@@ -11366,7 +11372,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>739</v>
       </c>
@@ -11412,7 +11418,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>739</v>
       </c>
@@ -11458,7 +11464,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="81" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="23" t="s">
         <v>739</v>
       </c>
@@ -11510,7 +11516,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>739</v>
       </c>
@@ -11556,7 +11562,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>739</v>
       </c>
@@ -11602,7 +11608,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>739</v>
       </c>
@@ -11648,7 +11654,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>739</v>
       </c>
@@ -11694,7 +11700,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="86" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" s="21" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="23" t="s">
         <v>739</v>
       </c>
@@ -11746,7 +11752,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>739</v>
       </c>
@@ -11792,7 +11798,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>804</v>
       </c>
@@ -11836,7 +11842,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>804</v>
       </c>
@@ -11936,7 +11942,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>804</v>
       </c>
@@ -11982,7 +11988,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>804</v>
       </c>
@@ -12086,7 +12092,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>804</v>
       </c>
@@ -12294,7 +12300,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>804</v>
       </c>
@@ -12344,7 +12350,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>804</v>
       </c>
@@ -12446,7 +12452,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>804</v>
       </c>
@@ -12496,35 +12502,37 @@
         <v>893</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="F104" s="19"/>
       <c r="G104" s="19"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="F105" s="19"/>
       <c r="G105" s="20"/>
       <c r="I105" s="19"/>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="F106" s="19"/>
       <c r="G106" s="20"/>
-      <c r="H106" s="31"/>
-      <c r="I106" s="32"/>
+      <c r="H106" s="43"/>
+      <c r="I106" s="44"/>
       <c r="J106" s="20"/>
       <c r="K106" s="19"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>894</v>
       </c>
       <c r="F107" s="19"/>
       <c r="G107" s="20"/>
-      <c r="H107" s="31"/>
-      <c r="I107" s="31"/>
-    </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H107" s="43"/>
+      <c r="I107" s="43"/>
+    </row>
+    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>715</v>
       </c>
@@ -12533,11 +12541,11 @@
       </c>
       <c r="F108" s="19"/>
       <c r="G108" s="20"/>
-      <c r="H108" s="31"/>
-      <c r="I108" s="31"/>
+      <c r="H108" s="43"/>
+      <c r="I108" s="43"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>896</v>
       </c>
@@ -12546,12 +12554,12 @@
       </c>
       <c r="F109" s="19"/>
       <c r="G109" s="20"/>
-      <c r="H109" s="31"/>
-      <c r="I109" s="32"/>
+      <c r="H109" s="43"/>
+      <c r="I109" s="44"/>
       <c r="J109" s="20"/>
       <c r="K109" s="19"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>898</v>
       </c>
@@ -12560,10 +12568,10 @@
       </c>
       <c r="F110" s="19"/>
       <c r="G110" s="20"/>
-      <c r="H110" s="31"/>
-      <c r="I110" s="31"/>
-    </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H110" s="43"/>
+      <c r="I110" s="43"/>
+    </row>
+    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>900</v>
       </c>
@@ -12572,11 +12580,11 @@
       </c>
       <c r="F111" s="19"/>
       <c r="G111" s="20"/>
-      <c r="H111" s="31"/>
-      <c r="I111" s="31"/>
+      <c r="H111" s="43"/>
+      <c r="I111" s="43"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>603</v>
       </c>
@@ -12585,12 +12593,12 @@
       </c>
       <c r="F112" s="19"/>
       <c r="G112" s="20"/>
-      <c r="H112" s="31"/>
-      <c r="I112" s="32"/>
+      <c r="H112" s="43"/>
+      <c r="I112" s="44"/>
       <c r="J112" s="20"/>
       <c r="K112" s="19"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>594</v>
       </c>
@@ -12599,118 +12607,136 @@
       </c>
       <c r="F113" s="19"/>
       <c r="G113" s="20"/>
-      <c r="H113" s="31"/>
-      <c r="I113" s="31"/>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H113" s="43"/>
+      <c r="I113" s="43"/>
+    </row>
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>729</v>
       </c>
       <c r="C114" t="s">
         <v>902</v>
       </c>
-      <c r="H114" s="31"/>
-      <c r="I114" s="31"/>
+      <c r="H114" s="43"/>
+      <c r="I114" s="43"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>882</v>
       </c>
       <c r="C115" t="s">
         <v>902</v>
       </c>
-      <c r="H115" s="31"/>
-      <c r="I115" s="32"/>
+      <c r="H115" s="43"/>
+      <c r="I115" s="44"/>
       <c r="J115" s="20"/>
       <c r="K115" s="19"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H116" s="31"/>
-      <c r="I116" s="31"/>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H117" s="31"/>
-      <c r="I117" s="31"/>
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H116" s="43"/>
+      <c r="I116" s="43"/>
+    </row>
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H117" s="43"/>
+      <c r="I117" s="43"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H118" s="31"/>
-      <c r="I118" s="32"/>
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H118" s="43"/>
+      <c r="I118" s="44"/>
       <c r="J118" s="20"/>
       <c r="K118" s="19"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H119" s="31"/>
-      <c r="I119" s="31"/>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H120" s="31"/>
-      <c r="I120" s="31"/>
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H119" s="43"/>
+      <c r="I119" s="43"/>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H120" s="43"/>
+      <c r="I120" s="43"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H121" s="31"/>
-      <c r="I121" s="32"/>
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H121" s="43"/>
+      <c r="I121" s="44"/>
       <c r="J121" s="20"/>
       <c r="K121" s="19"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H122" s="31"/>
-      <c r="I122" s="31"/>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H123" s="31"/>
-      <c r="I123" s="31"/>
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H122" s="43"/>
+      <c r="I122" s="43"/>
+    </row>
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H123" s="43"/>
+      <c r="I123" s="43"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H124" s="31"/>
-      <c r="I124" s="32"/>
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H124" s="43"/>
+      <c r="I124" s="44"/>
       <c r="J124" s="20"/>
       <c r="K124" s="19"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H125" s="31"/>
-      <c r="I125" s="31"/>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H126" s="31"/>
-      <c r="I126" s="31"/>
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H125" s="43"/>
+      <c r="I125" s="43"/>
+    </row>
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H126" s="43"/>
+      <c r="I126" s="43"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H127" s="31"/>
-      <c r="I127" s="32"/>
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H127" s="43"/>
+      <c r="I127" s="44"/>
       <c r="J127" s="20"/>
       <c r="K127" s="19"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-    </row>
-    <row r="129" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H129" s="31"/>
-      <c r="I129" s="31"/>
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H128" s="43"/>
+      <c r="I128" s="43"/>
+    </row>
+    <row r="129" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H129" s="43"/>
+      <c r="I129" s="43"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H130" s="31"/>
-      <c r="I130" s="32"/>
+    <row r="130" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H130" s="43"/>
+      <c r="I130" s="44"/>
       <c r="J130" s="20"/>
       <c r="K130" s="19"/>
     </row>
-    <row r="131" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H131" s="31"/>
-      <c r="I131" s="31"/>
-    </row>
-    <row r="132" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H132" s="31"/>
-      <c r="I132" s="31"/>
+    <row r="131" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H131" s="43"/>
+      <c r="I131" s="43"/>
+    </row>
+    <row r="132" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H132" s="43"/>
+      <c r="I132" s="43"/>
       <c r="K132" s="20"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R132" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Business"/>
+        <filter val="EU AI Act Compliance"/>
+        <filter val="Health &amp; Safety"/>
+        <filter val="Legal"/>
+        <filter val="Societal"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="12">
+      <filters>
+        <filter val="No"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="18">
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="I124:I126"/>
     <mergeCell ref="H106:H108"/>
     <mergeCell ref="H121:H123"/>
     <mergeCell ref="I106:I108"/>
@@ -12727,8 +12753,6 @@
     <mergeCell ref="H127:H129"/>
     <mergeCell ref="I127:I129"/>
     <mergeCell ref="H115:H117"/>
-    <mergeCell ref="H124:H126"/>
-    <mergeCell ref="I124:I126"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -15472,14 +15496,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="45" t="s">
         <v>1212</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -15804,14 +15828,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="45" t="s">
         <v>1284</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -16115,14 +16139,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="45" t="s">
         <v>1343</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">

</xml_diff>